<commit_message>
Updated the Excel version
</commit_message>
<xml_diff>
--- a/NeuralNets/NN.xlsx
+++ b/NeuralNets/NN.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27809"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Stuff/Courses/Projects/NeuralNets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ANN" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>X</t>
   </si>
@@ -87,6 +100,63 @@
   </si>
   <si>
     <t>dW1 (3rd Tr Ex.)</t>
+  </si>
+  <si>
+    <t>1st Tr Ex.</t>
+  </si>
+  <si>
+    <t>2nd Tr Ex.</t>
+  </si>
+  <si>
+    <t>3rd Tr Ex.</t>
+  </si>
+  <si>
+    <t>2ns TR Ex.</t>
+  </si>
+  <si>
+    <t>FORWARD PASS</t>
+  </si>
+  <si>
+    <t>Backward Pass</t>
+  </si>
+  <si>
+    <t>Yhat - Y</t>
+  </si>
+  <si>
+    <t>dW2 (1st Tr. Ex.)</t>
+  </si>
+  <si>
+    <t>dW2 (2nd Tr. Ex.)</t>
+  </si>
+  <si>
+    <t>dW2 (3rd Tr. Ex.)</t>
+  </si>
+  <si>
+    <t>dW2 (total)</t>
+  </si>
+  <si>
+    <t>W2*sigPrime(z2) 1st Tr. Ex.</t>
+  </si>
+  <si>
+    <t>W2*SigPrime(z2) 2nd Tr. Ex.</t>
+  </si>
+  <si>
+    <t>W2*SigPrime(z2) 3rd Tr. Ex.</t>
+  </si>
+  <si>
+    <t>dW1 1st Tr. Ex.</t>
+  </si>
+  <si>
+    <t>dW1 2nd Tr. Ex.</t>
+  </si>
+  <si>
+    <t>dW1 3rd Tr. Ex.</t>
+  </si>
+  <si>
+    <t>dW1 total</t>
+  </si>
+  <si>
+    <t>After one Epoch</t>
   </si>
 </sst>
 </file>
@@ -102,15 +172,45 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -120,44 +220,138 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -222,9 +416,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -257,9 +451,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -465,40 +659,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.75" customWidth="1"/>
-    <col min="10" max="10" width="9.625" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="J1" s="5" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="J1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="N1" s="5" t="s">
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="N1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -539,7 +734,7 @@
         <v>-0.10411428397546001</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -580,7 +775,7 @@
         <v>-0.67643580672679604</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -612,7 +807,7 @@
         <v>0.68237396694402497</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="N5" s="2">
         <v>0.51881553279291903</v>
       </c>
@@ -623,40 +818,41 @@
         <v>-0.16762477168312301</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="E7" s="5" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="E7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="J7" s="5" t="s">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="J7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="O7" s="5" t="s">
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="O7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="S7" s="5" t="s">
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="S7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="W7" s="5" t="s">
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="W7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f>(A2*J2)+(B2*K2)+(C2*L2)</f>
         <v>-0.14872375517481945</v>
@@ -665,6 +861,9 @@
         <f>(A2*J3)+(B2*K3)+(C2*L3)</f>
         <v>-0.82156201827130837</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E8" s="2">
         <f>(A13*N2)+(B13*O2)+(C13*P2)</f>
         <v>2.959180343765605E-2</v>
@@ -734,7 +933,7 @@
         <v>6.7364702475604277E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <f>(A3*J2)+(B3*K2)+(C3*L2)</f>
         <v>0.34051384109369687</v>
@@ -743,6 +942,9 @@
         <f>(A3*J3)+(B3*K3)+(C3*L3)</f>
         <v>-0.92696770105249982</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E9" s="2">
         <f>(A14*N2)+(B14*O2)+(C14*P2)</f>
         <v>7.5380079439604682E-3</v>
@@ -812,7 +1014,7 @@
         <v>3.7200249930355207E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <f>(A4*J2)+(B4*K2)+(C4*L2)</f>
         <v>-0.8322497422446844</v>
@@ -821,6 +1023,9 @@
         <f>(A4*J3)+(B4*K3)+(C4*L3)</f>
         <v>0.11605260986660293</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E10" s="2">
         <f>(A15*N2)+(B15*O2)+(C15*P2)</f>
         <v>3.8323233354842785E-2</v>
@@ -890,7 +1095,7 @@
         <v>-5.293922327926489E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="O11" s="2">
         <f>(M13*A13)</f>
         <v>-7.4546068470920338E-2</v>
@@ -928,31 +1133,31 @@
         <v>7.799083202284729E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="O12" s="5" t="s">
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="O12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -1009,7 +1214,7 @@
         <v>0.14167571267710266</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -1066,7 +1271,7 @@
         <v>1.8155985837554921E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>1</v>
       </c>
@@ -1123,7 +1328,7 @@
         <v>2.7649004184990257E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="O16" s="3">
         <f t="shared" si="8"/>
         <v>0.22089086704706862</v>
@@ -1137,32 +1342,32 @@
         <v>9.7186270709081909E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="13"/>
       <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="M17" s="5" t="s">
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="M17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="Q17" s="5" t="s">
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="Q17" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <f>B$13*(1-B$13)</f>
         <v>0.24862265811037962</v>
@@ -1216,7 +1421,7 @@
         <v>-8.6333511729384371E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <f>B$14*(1-B$14)</f>
         <v>0.24289092416946267</v>
@@ -1270,7 +1475,7 @@
         <v>-3.680244773452182E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <f>B$15*(1-B$15)</f>
         <v>0.21125778743734192</v>
@@ -1288,7 +1493,7 @@
         <v>0.45340248875491501</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D21" s="2">
         <f t="shared" si="15"/>
         <v>0.33274284027553469</v>
@@ -1297,13 +1502,13 @@
         <f t="shared" si="16"/>
         <v>-0.11137806003718306</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K21" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="K22" s="2">
         <f t="shared" ref="K22:M23" si="17">(I18+M18+Q18)</f>
         <v>1.138946839162615E-2</v>
@@ -1317,7 +1522,7 @@
         <v>-1.4012238264878817E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
@@ -1343,7 +1548,7 @@
         <v>-6.1165109628667128E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <f>($A$18*$O2)</f>
         <v>-4.9821735101567947E-2</v>
@@ -1369,7 +1574,7 @@
         <v>-2.594112779010592E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <f t="shared" ref="A25:A27" si="18">($A$18*$O3)</f>
         <v>-0.13401461463271849</v>
@@ -1395,7 +1600,7 @@
         <v>-0.16854082873238793</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <f t="shared" si="18"/>
         <v>2.6424993843269826E-2</v>
@@ -1421,7 +1626,7 @@
         <v>0.17002038146186321</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <f t="shared" si="18"/>
         <v>0.11771596422573795</v>
@@ -1447,14 +1652,14 @@
         <v>-4.1765408712258395E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G30" s="2">
         <f>(A24*J13)+(A25*K13)+(A26*L13)+(A27*M13)</f>
         <v>-2.154356531670288E-2</v>
@@ -1468,7 +1673,7 @@
         <v>-8.9914792125640568E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G31" s="2">
         <f>(B24*J13)+(B25*K13)+(B26*L13)+(B27*M13)</f>
         <v>8.8844455625981689E-3</v>
@@ -1484,24 +1689,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="J7:M7"/>
     <mergeCell ref="W7:Y7"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="E7:H7"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="A7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -1512,128 +1717,1246 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:J17"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:J5"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="116" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19:P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="10" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D4">
-        <v>0.7</v>
-      </c>
-      <c r="E4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F4">
-        <v>1.5</v>
-      </c>
-      <c r="H4">
-        <v>0.1</v>
-      </c>
-      <c r="I4">
-        <v>0.3</v>
-      </c>
-      <c r="J4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D5">
-        <v>0.8</v>
-      </c>
-      <c r="E5">
-        <v>1.2</v>
-      </c>
-      <c r="F5">
-        <v>1.6</v>
-      </c>
-      <c r="H5">
-        <v>0.2</v>
-      </c>
-      <c r="I5">
-        <v>0.4</v>
-      </c>
-      <c r="J5">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="D6">
-        <v>0.9</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="F6">
-        <v>1.7</v>
-      </c>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="D7">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="F7">
-        <v>1.8</v>
-      </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="J1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="N1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.54030230586813999</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-0.41614683654714202</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>-0.24629013174121001</v>
+      </c>
+      <c r="K2" s="2">
+        <v>-0.235801594600067</v>
+      </c>
+      <c r="L2" s="2">
+        <v>-0.54060370546804803</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0.15415011965877601</v>
+      </c>
+      <c r="O2" s="2">
+        <v>-0.20039096790385399</v>
+      </c>
+      <c r="P2" s="2">
+        <v>-0.10411428397546001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>-0.98999249660044497</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-0.65364362086361205</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>-0.52149209497043802</v>
+      </c>
+      <c r="K3" s="2">
+        <v>-3.5811923776202799E-2</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.67457116972511999</v>
+      </c>
+      <c r="N3" s="2">
+        <v>-0.222990663950239</v>
+      </c>
+      <c r="O3" s="2">
+        <v>-0.53902816280413501</v>
+      </c>
+      <c r="P3" s="2">
+        <v>-0.67643580672679604</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.28366218546322602</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.96017028665036597</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>-4.1001712383635397E-2</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.106285541487285</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.68237396694402497</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N5" s="3">
+        <v>0.51881553279291903</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.47347239033007299</v>
+      </c>
+      <c r="P5" s="3">
+        <v>-0.16762477168312301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <f>(A2*J2)+(B2*K2)+(C2*L2)</f>
+        <v>-0.14872375517481945</v>
+      </c>
+      <c r="B8" s="2">
+        <f>(A2*J3)+(B2*K3)+(C2*L3)</f>
+        <v>-0.82156201827130837</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <f>1/(1+EXP(-$A8))</f>
+        <v>0.46288744296575141</v>
+      </c>
+      <c r="F8" s="2">
+        <f>1/(1+EXP(-$B8))</f>
+        <v>0.30543218740445194</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="2">
+        <f>($D8*$N$2)+($E8*$O$2)+($F8*$P$2)</f>
+        <v>2.959180343765605E-2</v>
+      </c>
+      <c r="I8" s="2">
+        <f>($D8*$N$3)+($E8*$O$3)+($F8*$P$3)</f>
+        <v>-0.67910530000443226</v>
+      </c>
+      <c r="J8" s="2">
+        <f>($D8*$N$4)+($E8*$O$4)+($F8*$P$4)</f>
+        <v>0.21661550349121098</v>
+      </c>
+      <c r="K8" s="2">
+        <f>($D8*$N$5)+($E8*$O$5)+($F8*$P$5)</f>
+        <v>0.68678195618934057</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="2">
+        <f>(1/(1+EXP(-$H8)))</f>
+        <v>0.50739741105673586</v>
+      </c>
+      <c r="N8" s="2">
+        <f>(1/(1+EXP(-$I8)))</f>
+        <v>0.33646101960926972</v>
+      </c>
+      <c r="O8" s="2">
+        <f>(1/(1+EXP(-$J8)))</f>
+        <v>0.55394311283828446</v>
+      </c>
+      <c r="P8" s="2">
+        <f>(1/(1+EXP(-$K8)))</f>
+        <v>0.66525067495879964</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <f>(A3*J2)+(B3*K2)+(C3*L2)</f>
+        <v>0.34051384109369687</v>
+      </c>
+      <c r="B9" s="2">
+        <f>(A3*J3)+(B3*K3)+(C3*L3)</f>
+        <v>-0.92696770105249982</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <f>1/(1+EXP(-$A9))</f>
+        <v>0.584315335678258</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" ref="F9:F10" si="0">1/(1+EXP(-$B9))</f>
+        <v>0.28354030695867</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" ref="H9:H10" si="1">($D9*$N$2)+($E9*$O$2)+($F9*$P$2)</f>
+        <v>7.5380079439604682E-3</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" ref="I9:I10" si="2">($D9*$N$3)+($E9*$O$3)+($F9*$P$3)</f>
+        <v>-0.72974990211632318</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" ref="J9:J10" si="3">($D9*$N$4)+($E9*$O$4)+($F9*$P$4)</f>
+        <v>0.21458308351616712</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" ref="K9:K10" si="4">($D9*$N$5)+($E9*$O$5)+($F9*$P$5)</f>
+        <v>0.74794433226611323</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" ref="M9:M10" si="5">(1/(1+EXP(-$H9)))</f>
+        <v>0.50188449306267835</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" ref="N9:N10" si="6">(1/(1+EXP(-$I9)))</f>
+        <v>0.32524961207593989</v>
+      </c>
+      <c r="O9" s="2">
+        <f>(1/(1+EXP(-$J9)))</f>
+        <v>0.553440867010074</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" ref="P9:P10" si="7">(1/(1+EXP(-$K9)))</f>
+        <v>0.67873061458129647</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <f>(A4*J2)+(B4*K2)+(C4*L2)</f>
+        <v>-0.8322497422446844</v>
+      </c>
+      <c r="B10" s="2">
+        <f>(A4*J3)+(B4*K3)+(C4*L3)</f>
+        <v>0.11605260986660293</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <f>1/(1+EXP(-$A10))</f>
+        <v>0.3031695842542162</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52898063333176271</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>3.8323233354842785E-2</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.74422904941950496</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="3"/>
+        <v>0.35218344424445669</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="4"/>
+        <v>0.57368770263810676</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="5"/>
+        <v>0.50957963592357947</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="6"/>
+        <v>0.32208006016859186</v>
+      </c>
+      <c r="O10" s="2">
+        <f>(1/(1+EXP(-$J10)))</f>
+        <v>0.58714695812981244</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="7"/>
+        <v>0.63961365711710727</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="J17" s="1"/>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="K14" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <f>(M$8-E$2)</f>
+        <v>0.50739741105673586</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" ref="B15:D15" si="8">(N$8-F$2)</f>
+        <v>0.33646101960926972</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="8"/>
+        <v>0.55394311283828446</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="8"/>
+        <v>-0.33474932504120036</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="2">
+        <f>M$8*(1-M$8)</f>
+        <v>0.24994527830965768</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" ref="G15:I15" si="9">N$8*(1-N$8)</f>
+        <v>0.22325500189276035</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="9"/>
+        <v>0.2470901405773161</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="9"/>
+        <v>0.22269221442566114</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="2">
+        <f>A$15*F$15</f>
+        <v>0.12682158712017563</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" ref="L15:N15" si="10">B$15*G$15</f>
+        <v>7.511660556970759E-2</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="10"/>
+        <v>0.13687388162304778</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="10"/>
+        <v>-7.4546068470920338E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <f>(M$9-E$3)</f>
+        <v>0.50188449306267835</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" ref="B16:D16" si="11">(N$9-F$3)</f>
+        <v>-0.67475038792406017</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="11"/>
+        <v>0.553440867010074</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="11"/>
+        <v>0.67873061458129647</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="2">
+        <f>M$9*(1-M$9)</f>
+        <v>0.24999644868589671</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" ref="G16:I16" si="12">N$9*(1-N$9)</f>
+        <v>0.21946230192039051</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="12"/>
+        <v>0.24714407373321159</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="12"/>
+        <v>0.21805536741139206</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="2">
+        <f>A$16*F$16</f>
+        <v>0.12546934091619116</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" ref="L16:N16" si="13">B$16*G$16</f>
+        <v>-0.14808227335549071</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="13"/>
+        <v>0.13677963044331029</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="13"/>
+        <v>0.14800085353588455</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <f>(M$10-E$4)</f>
+        <v>0.50957963592357947</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" ref="B17:D17" si="14">(N$10-F$4)</f>
+        <v>0.32208006016859186</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="14"/>
+        <v>-0.41285304187018756</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="14"/>
+        <v>0.63961365711710727</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="2">
+        <f>M$10*(1-M$10)</f>
+        <v>0.24990823057557165</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" ref="G17:I17" si="15">N$10*(1-N$10)</f>
+        <v>0.21834449501038813</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="15"/>
+        <v>0.24240540768872071</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="15"/>
+        <v>0.23050802674638679</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" s="11">
+        <f>A$17*F$17</f>
+        <v>0.12734814515100576</v>
+      </c>
+      <c r="L17" s="11">
+        <f t="shared" ref="L17:N17" si="16">B$17*G$17</f>
+        <v>7.0324408090426616E-2</v>
+      </c>
+      <c r="M17" s="11">
+        <f t="shared" si="16"/>
+        <v>-0.1000778099300713</v>
+      </c>
+      <c r="N17" s="11">
+        <f t="shared" si="16"/>
+        <v>0.14743608198210442</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="E19" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="I19" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="M19" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <f>K15*D8</f>
+        <v>0.12682158712017563</v>
+      </c>
+      <c r="B20" s="2">
+        <f>K15*E8</f>
+        <v>5.8704120174916372E-2</v>
+      </c>
+      <c r="C20" s="2">
+        <f>K15*F8</f>
+        <v>3.8735394764219513E-2</v>
+      </c>
+      <c r="E20" s="2">
+        <f>K16*D9</f>
+        <v>0.12546934091619116</v>
+      </c>
+      <c r="F20" s="2">
+        <f>K16*E9</f>
+        <v>7.3313660054774035E-2</v>
+      </c>
+      <c r="G20" s="2">
+        <f>K16*F9</f>
+        <v>3.5575615437278857E-2</v>
+      </c>
+      <c r="I20" s="2">
+        <f>K17*D10</f>
+        <v>0.12734814515100576</v>
+      </c>
+      <c r="J20" s="2">
+        <f>K17*E10</f>
+        <v>3.8608084220975995E-2</v>
+      </c>
+      <c r="K20" s="2">
+        <f>K17*F10</f>
+        <v>6.7364702475604277E-2</v>
+      </c>
+      <c r="M20" s="20">
+        <f>$A20+$E20+$I20</f>
+        <v>0.37963907318737256</v>
+      </c>
+      <c r="N20" s="20">
+        <f>$B20+$F20+$J20</f>
+        <v>0.17062586445066641</v>
+      </c>
+      <c r="O20" s="20">
+        <f>$C20+$G20+$K20</f>
+        <v>0.14167571267710266</v>
+      </c>
+      <c r="P20" s="22"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <f>L15*D8</f>
+        <v>7.511660556970759E-2</v>
+      </c>
+      <c r="B21" s="2">
+        <f>L15*E8</f>
+        <v>3.4770533476428868E-2</v>
+      </c>
+      <c r="C21" s="2">
+        <f>L15*F8</f>
+        <v>2.2943029149553228E-2</v>
+      </c>
+      <c r="E21" s="2">
+        <f>L16*D9</f>
+        <v>-0.14808227335549071</v>
+      </c>
+      <c r="F21" s="2">
+        <f>L16*E9</f>
+        <v>-8.652674326371311E-2</v>
+      </c>
+      <c r="G21" s="2">
+        <f>L16*F9</f>
+        <v>-4.1987293242353514E-2</v>
+      </c>
+      <c r="I21" s="2">
+        <f>L17*D10</f>
+        <v>7.0324408090426616E-2</v>
+      </c>
+      <c r="J21" s="2">
+        <f>L17*E10</f>
+        <v>2.1320221563698474E-2</v>
+      </c>
+      <c r="K21" s="2">
+        <f>L17*F10</f>
+        <v>3.7200249930355207E-2</v>
+      </c>
+      <c r="M21" s="20">
+        <f t="shared" ref="M21:M23" si="17">$A21+$E21+$I21</f>
+        <v>-2.6412596953565015E-3</v>
+      </c>
+      <c r="N21" s="20">
+        <f t="shared" ref="N21:N23" si="18">$B21+$F21+$J21</f>
+        <v>-3.0435988223585769E-2</v>
+      </c>
+      <c r="O21" s="20">
+        <f t="shared" ref="O21:O23" si="19">$C21+$G21+$K21</f>
+        <v>1.8155985837554921E-2</v>
+      </c>
+      <c r="P21" s="22"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <f>M15*D8</f>
+        <v>0.13687388162304778</v>
+      </c>
+      <c r="B22" s="2">
+        <f>M15*E8</f>
+        <v>6.3357201073289543E-2</v>
+      </c>
+      <c r="C22" s="2">
+        <f>M15*F8</f>
+        <v>4.1805689062665498E-2</v>
+      </c>
+      <c r="E22" s="2">
+        <f>M16*D9</f>
+        <v>0.13677963044331029</v>
+      </c>
+      <c r="F22" s="2">
+        <f>M16*E9</f>
+        <v>7.9922435676430925E-2</v>
+      </c>
+      <c r="G22" s="2">
+        <f>M16*F9</f>
+        <v>3.8782538401589642E-2</v>
+      </c>
+      <c r="I22" s="2">
+        <f>M17*D10</f>
+        <v>-0.1000778099300713</v>
+      </c>
+      <c r="J22" s="2">
+        <f>M17*E10</f>
+        <v>-3.0340548029572187E-2</v>
+      </c>
+      <c r="K22" s="2">
+        <f>M17*F10</f>
+        <v>-5.293922327926489E-2</v>
+      </c>
+      <c r="M22" s="20">
+        <f t="shared" si="17"/>
+        <v>0.17357570213628676</v>
+      </c>
+      <c r="N22" s="20">
+        <f t="shared" si="18"/>
+        <v>0.11293908872014828</v>
+      </c>
+      <c r="O22" s="20">
+        <f t="shared" si="19"/>
+        <v>2.7649004184990257E-2</v>
+      </c>
+      <c r="P22" s="22"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <f>N15*D8</f>
+        <v>-7.4546068470920338E-2</v>
+      </c>
+      <c r="B23" s="2">
+        <f>N15*E8</f>
+        <v>-3.4506439017654135E-2</v>
+      </c>
+      <c r="C23" s="2">
+        <f>N15*F8</f>
+        <v>-2.2768768755475247E-2</v>
+      </c>
+      <c r="E23" s="2">
+        <f>N16*D9</f>
+        <v>0.14800085353588455</v>
+      </c>
+      <c r="F23" s="2">
+        <f>N16*E9</f>
+        <v>8.6479168414489077E-2</v>
+      </c>
+      <c r="G23" s="2">
+        <f>N16*F9</f>
+        <v>4.1964207441709866E-2</v>
+      </c>
+      <c r="I23" s="2">
+        <f>N17*D10</f>
+        <v>0.14743608198210442</v>
+      </c>
+      <c r="J23" s="2">
+        <f>N17*E10</f>
+        <v>4.4698135678585132E-2</v>
+      </c>
+      <c r="K23" s="2">
+        <f>N17*F10</f>
+        <v>7.799083202284729E-2</v>
+      </c>
+      <c r="M23" s="20">
+        <f t="shared" si="17"/>
+        <v>0.22089086704706862</v>
+      </c>
+      <c r="N23" s="20">
+        <f t="shared" si="18"/>
+        <v>9.6670865075420082E-2</v>
+      </c>
+      <c r="O23" s="20">
+        <f t="shared" si="19"/>
+        <v>9.7186270709081909E-2</v>
+      </c>
+      <c r="P23" s="22"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="E25" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="H25" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I25" s="17"/>
+      <c r="K25" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L25" s="17"/>
+      <c r="N25" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O25" s="17"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <f t="shared" ref="A26:B28" si="20">E8*(1-E8)</f>
+        <v>0.24862265811037962</v>
+      </c>
+      <c r="B26" s="2">
+        <f t="shared" si="20"/>
+        <v>0.21214336630178371</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="2">
+        <f>(A26*O2)</f>
+        <v>-4.9821735101567947E-2</v>
+      </c>
+      <c r="F26" s="2">
+        <f>B26*P2</f>
+        <v>-2.2087154682653942E-2</v>
+      </c>
+      <c r="H26" s="2">
+        <f>A27*O2</f>
+        <v>-4.8673147389380229E-2</v>
+      </c>
+      <c r="I26" s="2">
+        <f>B27*P2</f>
+        <v>-2.1150317175198E-2</v>
+      </c>
+      <c r="K26" s="2">
+        <f>A28*O2</f>
+        <v>-4.2334152501795591E-2</v>
+      </c>
+      <c r="L26" s="2">
+        <f>B28*P2</f>
+        <v>-2.594112779010592E-2</v>
+      </c>
+      <c r="N26" s="2">
+        <f>$E26+$H26+$K26</f>
+        <v>-0.14082903499274377</v>
+      </c>
+      <c r="O26" s="2">
+        <f>$F26+$I26+$L26</f>
+        <v>-6.9178599647957861E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <f t="shared" si="20"/>
+        <v>0.24289092416946267</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" si="20"/>
+        <v>0.2031452012884532</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="2">
+        <f>A26*O3</f>
+        <v>-0.13401461463271849</v>
+      </c>
+      <c r="F27" s="2">
+        <f>B26*P3</f>
+        <v>-0.14350136912608527</v>
+      </c>
+      <c r="H27" s="2">
+        <f>A27*O3</f>
+        <v>-0.13092504861686394</v>
+      </c>
+      <c r="I27" s="2">
+        <f>B27*P3</f>
+        <v>-0.1374146881162322</v>
+      </c>
+      <c r="K27" s="2">
+        <f>A28*O3</f>
+        <v>-0.11387389704041688</v>
+      </c>
+      <c r="L27" s="2">
+        <f>B28*P3</f>
+        <v>-0.16854082873238793</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" ref="N27:N29" si="21">$E27+$H27+$K27</f>
+        <v>-0.3788135602899993</v>
+      </c>
+      <c r="O27" s="2">
+        <f t="shared" ref="O27:O29" si="22">$F27+$I27+$L27</f>
+        <v>-0.44945688597470546</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <f t="shared" si="20"/>
+        <v>0.21125778743734192</v>
+      </c>
+      <c r="B28" s="2">
+        <f t="shared" si="20"/>
+        <v>0.24916012289168993</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="2">
+        <f>A26*O4</f>
+        <v>2.6424993843269826E-2</v>
+      </c>
+      <c r="F28" s="2">
+        <f>B26*P4</f>
+        <v>0.14476111042420753</v>
+      </c>
+      <c r="H28" s="2">
+        <f>A27*O4</f>
+        <v>2.5815793397698419E-2</v>
+      </c>
+      <c r="I28" s="2">
+        <f>B27*P4</f>
+        <v>0.13862099686884427</v>
+      </c>
+      <c r="K28" s="2">
+        <f>A28*O4</f>
+        <v>2.2453648331183639E-2</v>
+      </c>
+      <c r="L28" s="2">
+        <f>B28*P4</f>
+        <v>0.17002038146186321</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="21"/>
+        <v>7.4694435572151885E-2</v>
+      </c>
+      <c r="O28" s="2">
+        <f t="shared" si="22"/>
+        <v>0.45340248875491501</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E29" s="2">
+        <f>A26*O5</f>
+        <v>0.11771596422573795</v>
+      </c>
+      <c r="F29" s="2">
+        <f>B26*P5</f>
+        <v>-3.5560483340425629E-2</v>
+      </c>
+      <c r="H29" s="2">
+        <f>A27*O5</f>
+        <v>0.11500214645599599</v>
+      </c>
+      <c r="I29" s="2">
+        <f>B27*P5</f>
+        <v>-3.4052167984499032E-2</v>
+      </c>
+      <c r="K29" s="2">
+        <f>A28*O5</f>
+        <v>0.10002472959380074</v>
+      </c>
+      <c r="L29" s="2">
+        <f>B28*P5</f>
+        <v>-4.1765408712258395E-2</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="21"/>
+        <v>0.33274284027553469</v>
+      </c>
+      <c r="O29" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.11137806003718306</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <f>(E26*K15)+(E27*L15)+(E28*M15)+(E29*N15)</f>
+        <v>-2.154356531670288E-2</v>
+      </c>
+      <c r="B31" s="2">
+        <f>(H26*K16)+(H27*L16)+(H28*M16)+(H29*N16)</f>
+        <v>3.3832181629585435E-2</v>
+      </c>
+      <c r="C31" s="2">
+        <f>(K26*K17)+(K27*L17)+(K28*M17)+(K29*N17)</f>
+        <v>-8.9914792125640568E-4</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="I31" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="M31" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <f>(F26*K15)+(F27*L15)+(F28*M15)+(F29*N15)</f>
+        <v>8.8844455625981689E-3</v>
+      </c>
+      <c r="B32" s="2">
+        <f>(I26*K16)+(I27*L16)+(I28*M16)+(I29*N16)</f>
+        <v>3.1615741849497517E-2</v>
+      </c>
+      <c r="C32" s="2">
+        <f>(L26*K17)+(L27*L17)+(L28*M17)+(L29*N17)</f>
+        <v>-3.8329084169965541E-2</v>
+      </c>
+      <c r="E32" s="2">
+        <f>A$2*$A$31</f>
+        <v>-2.154356531670288E-2</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" ref="F32:G32" si="23">B$2*$A$31</f>
+        <v>-1.1640038017235451E-2</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="23"/>
+        <v>8.9652865544926318E-3</v>
+      </c>
+      <c r="I32" s="2">
+        <f>A3*B31</f>
+        <v>3.3832181629585435E-2</v>
+      </c>
+      <c r="J32" s="2">
+        <f>B3*B31</f>
+        <v>-3.3493605956912996E-2</v>
+      </c>
+      <c r="K32" s="2">
+        <f>C3*B31</f>
+        <v>-2.2114189702077604E-2</v>
+      </c>
+      <c r="M32" s="2">
+        <f>A4*C31</f>
+        <v>-8.9914792125640568E-4</v>
+      </c>
+      <c r="N32" s="2">
+        <f>B4*C31</f>
+        <v>-2.550542643983087E-4</v>
+      </c>
+      <c r="O32" s="2">
+        <f>C4*C31</f>
+        <v>-8.6333511729384371E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E33" s="2">
+        <f>(A2*A32)</f>
+        <v>8.8844455625981689E-3</v>
+      </c>
+      <c r="F33" s="2">
+        <f>B2*A32</f>
+        <v>4.8002864238317552E-3</v>
+      </c>
+      <c r="G33" s="2">
+        <f>C2*A32</f>
+        <v>-3.6972339153505214E-3</v>
+      </c>
+      <c r="I33" s="2">
+        <f>A3*B32</f>
+        <v>3.1615741849497517E-2</v>
+      </c>
+      <c r="J33" s="2">
+        <f>B3*B32</f>
+        <v>-3.1299347205459217E-2</v>
+      </c>
+      <c r="K33" s="2">
+        <f>C3*B32</f>
+        <v>-2.0665427978794788E-2</v>
+      </c>
+      <c r="M33" s="2">
+        <f>A4*C32</f>
+        <v>-3.8329084169965541E-2</v>
+      </c>
+      <c r="N33" s="2">
+        <f>B4*C32</f>
+        <v>-1.0872511782456367E-2</v>
+      </c>
+      <c r="O33" s="2">
+        <f>C4*C32</f>
+        <v>-3.680244773452182E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="20">
+        <f>E32+I32+M32</f>
+        <v>1.138946839162615E-2</v>
+      </c>
+      <c r="B36" s="20">
+        <f>F32+J32+N32</f>
+        <v>-4.538869823854675E-2</v>
+      </c>
+      <c r="C36" s="20">
+        <f>G32+K32+O32</f>
+        <v>-1.4012238264878817E-2</v>
+      </c>
+      <c r="D36" s="22"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="20">
+        <f>E33+I33+M33</f>
+        <v>2.1711032421301429E-3</v>
+      </c>
+      <c r="B37" s="20">
+        <f>F33+J33+N33</f>
+        <v>-3.7371572564083827E-2</v>
+      </c>
+      <c r="C37" s="20">
+        <f>G33+K33+O33</f>
+        <v>-6.1165109628667128E-2</v>
+      </c>
+      <c r="D37" s="22"/>
     </row>
   </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="P19:P23"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A13:P13"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A6:P6"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="N25:O25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>